<commit_message>
Final; changes on self evaluation
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheBestMum\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Nasko\megdan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18990" windowHeight="9345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -647,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1111,9 @@
       <c r="D42" s="7">
         <v>20</v>
       </c>
-      <c r="E42" s="7"/>
+      <c r="E42" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">

</xml_diff>